<commit_message>
CRUD Ride & Ride Queue, Store UI, Customer UI (View Stores), Diagrams [INITIAL]
</commit_message>
<xml_diff>
--- a/diagrams/MJ_VorteKia_UseCaseDescriptions.xlsx
+++ b/diagrams/MJ_VorteKia_UseCaseDescriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\S-1 BINUS\SLC\TPA-Desktop\MJ_VorteKia_Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAA417E-DA47-4DF5-961D-DA0125DF40C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E192CFEF-2F29-4D3B-A429-F020A4695B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" xr2:uid="{2183EE87-2FE0-1848-A8EC-EAF6DA5552F2}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="30936" windowHeight="16896" xr2:uid="{2183EE87-2FE0-1848-A8EC-EAF6DA5552F2}"/>
   </bookViews>
   <sheets>
     <sheet name="VorteKia Use Case Descriptions" sheetId="1" r:id="rId1"/>
@@ -909,9 +909,6 @@
 6.2 If updating the database fails due to a database issue, rolls back the transaction and displays an error message ("Top-up could not be completed. Please try again later.") and stops further processing.</t>
   </si>
   <si>
-    <t xml:space="preserve">	2.1 The UI renders the form with clear instructions, indicating that the amount must be a positive numeric value (greater than 0) less than the max top-up limit (Rp 10.000.000) and that a valid payment method must be selected.</t>
-  </si>
-  <si>
     <t>5.1 Input Validations:
     5.1.1 Validates that the top-up amount field is not empty.
     5.1.2 Validates that the input is numeric.
@@ -1162,6 +1159,9 @@
     <t>5.1 If the selected MaintenanceRequestdoes not exist or is already assigned, displays an error message ("Select a valid, unassigned request.") and stops further processing.
 5.1 If the chosen Maintenance Staff is not available, displays an error message ("Staff is not available. Please choose another staff member.") and stops further processing.
 5.2 If updating the database fails due to a database issue, rolls back the transaction and displays an error message ("Assigning maintenance request could not be completed. Please try again later.") and stops further processing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	2.1 The UI renders the form with clear instructions, indicating that the amount must be a positive numeric value (greater than 0) less than the max top-up limit (Rp 1.000.000) and that a valid payment method must be selected.</t>
   </si>
 </sst>
 </file>
@@ -1299,10 +1299,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1621,27 +1621,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3915B7-9862-624A-8796-A82526CFDDED}">
   <dimension ref="B2:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94:D94"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.19921875" customWidth="1"/>
+    <col min="3" max="3" width="50.796875" customWidth="1"/>
     <col min="4" max="4" width="53.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="2:4" ht="64.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="D5" s="12"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B12" s="10"/>
       <c r="C12" s="2" t="s">
         <v>20</v>
@@ -1733,16 +1733,16 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="2" t="s">
         <v>22</v>
@@ -1751,7 +1751,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="2" t="s">
         <v>23</v>
@@ -1760,16 +1760,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="124" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" ht="124.8" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
       <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="108.5" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
       <c r="C17" s="2" t="s">
         <v>25</v>
@@ -1778,7 +1778,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
       <c r="C18" s="2" t="s">
         <v>26</v>
@@ -1787,7 +1787,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="156.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" ht="156.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>12</v>
       </c>
@@ -1796,16 +1796,16 @@
       </c>
       <c r="D19" s="12"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>8</v>
       </c>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="2:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="D24" s="12"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
@@ -1841,16 +1841,16 @@
       </c>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
         <v>11</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B31" s="10"/>
       <c r="C31" s="2" t="s">
         <v>37</v>
@@ -1897,7 +1897,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B32" s="10"/>
       <c r="C32" s="2" t="s">
         <v>38</v>
@@ -1906,7 +1906,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B33" s="10"/>
       <c r="C33" s="2" t="s">
         <v>39</v>
@@ -1915,7 +1915,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B34" s="10"/>
       <c r="C34" s="2" t="s">
         <v>40</v>
@@ -1924,16 +1924,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="155" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:4" ht="156" x14ac:dyDescent="0.3">
       <c r="B35" s="10"/>
       <c r="C35" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B36" s="10"/>
       <c r="C36" s="2" t="s">
         <v>41</v>
@@ -1942,25 +1942,25 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="112.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:4" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D37" s="12"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="14"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>0</v>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>8</v>
       </c>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="D41" s="9"/>
     </row>
-    <row r="42" spans="2:4" ht="82.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>9</v>
       </c>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="D42" s="12"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>1</v>
       </c>
@@ -1996,16 +1996,16 @@
       </c>
       <c r="D43" s="9"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="14" t="s">
         <v>61</v>
       </c>
       <c r="D44" s="9"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>2</v>
       </c>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>3</v>
       </c>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>4</v>
       </c>
@@ -2032,7 +2032,7 @@
       </c>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
         <v>11</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B49" s="10"/>
       <c r="C49" s="2" t="s">
         <v>53</v>
@@ -2052,7 +2052,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B50" s="10"/>
       <c r="C50" s="2" t="s">
         <v>55</v>
@@ -2061,7 +2061,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B51" s="10"/>
       <c r="C51" s="2" t="s">
         <v>57</v>
@@ -2070,7 +2070,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B52" s="10"/>
       <c r="C52" s="2" t="s">
         <v>40</v>
@@ -2079,7 +2079,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="2:4" ht="155" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:4" ht="140.4" x14ac:dyDescent="0.3">
       <c r="B53" s="10"/>
       <c r="C53" s="2" t="s">
         <v>24</v>
@@ -2088,7 +2088,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="2:4" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="B54" s="10"/>
       <c r="C54" s="2" t="s">
         <v>60</v>
@@ -2097,7 +2097,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="2:4" ht="97.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="4" t="s">
         <v>12</v>
       </c>
@@ -2106,16 +2106,16 @@
       </c>
       <c r="D55" s="12"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D57" s="14"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D57" s="13"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
         <v>0</v>
       </c>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="D58" s="9"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>8</v>
       </c>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="D59" s="9"/>
     </row>
-    <row r="60" spans="2:4" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:4" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>9</v>
       </c>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="D60" s="12"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>1</v>
       </c>
@@ -2151,16 +2151,16 @@
       </c>
       <c r="D61" s="9"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="14" t="s">
         <v>66</v>
       </c>
       <c r="D62" s="9"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>2</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="D63" s="9"/>
     </row>
-    <row r="64" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>3</v>
       </c>
@@ -2178,7 +2178,7 @@
       </c>
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
         <v>4</v>
       </c>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="D65" s="5"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" s="10" t="s">
         <v>11</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B67" s="10"/>
       <c r="C67" s="2" t="s">
         <v>71</v>
@@ -2207,7 +2207,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B68" s="10"/>
       <c r="C68" s="2" t="s">
         <v>72</v>
@@ -2216,7 +2216,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B69" s="10"/>
       <c r="C69" s="2" t="s">
         <v>73</v>
@@ -2225,7 +2225,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B70" s="10"/>
       <c r="C70" s="2" t="s">
         <v>74</v>
@@ -2234,16 +2234,16 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="2:4" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="B71" s="10"/>
       <c r="C71" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B72" s="10"/>
       <c r="C72" s="2" t="s">
         <v>75</v>
@@ -2252,7 +2252,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="2:4" ht="97.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="4" t="s">
         <v>12</v>
       </c>
@@ -2261,43 +2261,43 @@
       </c>
       <c r="D73" s="12"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="D75" s="14"/>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C75" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D75" s="13"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D76" s="9"/>
     </row>
-    <row r="77" spans="2:4" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D77" s="9"/>
     </row>
-    <row r="78" spans="2:4" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:4" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D78" s="12"/>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
         <v>1</v>
       </c>
@@ -2306,16 +2306,16 @@
       </c>
       <c r="D79" s="9"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="13" t="s">
-        <v>173</v>
+      <c r="C80" s="14" t="s">
+        <v>172</v>
       </c>
       <c r="D80" s="9"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
         <v>2</v>
       </c>
@@ -2324,25 +2324,25 @@
       </c>
       <c r="D81" s="9"/>
     </row>
-    <row r="82" spans="2:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D82" s="7"/>
     </row>
-    <row r="83" spans="2:4" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D83" s="5"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" s="10" t="s">
         <v>11</v>
       </c>
@@ -2353,79 +2353,79 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B85" s="10"/>
       <c r="C85" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B86" s="10"/>
       <c r="C86" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B87" s="10"/>
       <c r="C87" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B88" s="10"/>
       <c r="C88" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" ht="170.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="2:4" ht="171.6" x14ac:dyDescent="0.3">
       <c r="B89" s="10"/>
       <c r="C89" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" ht="124" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" ht="124.8" x14ac:dyDescent="0.3">
       <c r="B90" s="10"/>
       <c r="C90" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D91" s="12"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C93" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D93" s="14"/>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D93" s="13"/>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
         <v>0</v>
       </c>
@@ -2434,7 +2434,7 @@
       </c>
       <c r="D94" s="9"/>
     </row>
-    <row r="95" spans="2:4" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
         <v>8</v>
       </c>
@@ -2443,7 +2443,7 @@
       </c>
       <c r="D95" s="9"/>
     </row>
-    <row r="96" spans="2:4" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:4" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
         <v>9</v>
       </c>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="D96" s="12"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
         <v>1</v>
       </c>
@@ -2461,16 +2461,16 @@
       </c>
       <c r="D97" s="9"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C98" s="13" t="s">
+      <c r="C98" s="14" t="s">
         <v>88</v>
       </c>
       <c r="D98" s="9"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99" s="1" t="s">
         <v>2</v>
       </c>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="D99" s="9"/>
     </row>
-    <row r="100" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B100" s="1" t="s">
         <v>3</v>
       </c>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="D100" s="7"/>
     </row>
-    <row r="101" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B101" s="1" t="s">
         <v>4</v>
       </c>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="D101" s="5"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102" s="10" t="s">
         <v>11</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="2:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B103" s="10"/>
       <c r="C103" s="2" t="s">
         <v>91</v>
@@ -2517,7 +2517,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="104" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B104" s="10"/>
       <c r="C104" s="2" t="s">
         <v>92</v>
@@ -2526,7 +2526,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="105" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B105" s="10"/>
       <c r="C105" s="2" t="s">
         <v>93</v>
@@ -2535,7 +2535,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="106" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B106" s="10"/>
       <c r="C106" s="2" t="s">
         <v>40</v>
@@ -2544,7 +2544,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="107" spans="2:4" ht="170.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:4" ht="171.6" x14ac:dyDescent="0.3">
       <c r="B107" s="10"/>
       <c r="C107" s="2" t="s">
         <v>24</v>
@@ -2553,7 +2553,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="2:4" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="B108" s="10"/>
       <c r="C108" s="2" t="s">
         <v>94</v>
@@ -2562,7 +2562,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="109" spans="2:4" ht="144.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:4" ht="144.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="4" t="s">
         <v>12</v>
       </c>
@@ -2571,16 +2571,16 @@
       </c>
       <c r="D109" s="12"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B111" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C111" s="14" t="s">
+      <c r="C111" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D111" s="14"/>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D111" s="13"/>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B112" s="1" t="s">
         <v>0</v>
       </c>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="D112" s="9"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B113" s="1" t="s">
         <v>8</v>
       </c>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="D113" s="9"/>
     </row>
-    <row r="114" spans="2:4" ht="64.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="1" t="s">
         <v>9</v>
       </c>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="D114" s="12"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B115" s="1" t="s">
         <v>1</v>
       </c>
@@ -2616,16 +2616,16 @@
       </c>
       <c r="D115" s="9"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B116" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D116" s="9"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B117" s="1" t="s">
         <v>2</v>
       </c>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="D117" s="9"/>
     </row>
-    <row r="118" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B118" s="1" t="s">
         <v>3</v>
       </c>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="D118" s="7"/>
     </row>
-    <row r="119" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
         <v>4</v>
       </c>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="D119" s="5"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B120" s="10" t="s">
         <v>11</v>
       </c>
@@ -2663,16 +2663,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="2:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B121" s="10"/>
       <c r="C121" s="2" t="s">
         <v>115</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="122" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B122" s="10"/>
       <c r="C122" s="2" t="s">
         <v>116</v>
@@ -2681,7 +2681,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B123" s="10"/>
       <c r="C123" s="2" t="s">
         <v>118</v>
@@ -2690,7 +2690,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="124" spans="2:4" ht="93" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:4" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B124" s="10"/>
       <c r="C124" s="2" t="s">
         <v>120</v>
@@ -2699,7 +2699,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="125" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B125" s="10"/>
       <c r="C125" s="2" t="s">
         <v>121</v>
@@ -2708,7 +2708,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="126" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B126" s="10"/>
       <c r="C126" s="2" t="s">
         <v>122</v>
@@ -2717,7 +2717,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="127" spans="2:4" ht="155" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:4" ht="156" x14ac:dyDescent="0.3">
       <c r="B127" s="10"/>
       <c r="C127" s="2" t="s">
         <v>123</v>
@@ -2726,7 +2726,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="128" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B128" s="10"/>
       <c r="C128" s="2" t="s">
         <v>124</v>
@@ -2735,7 +2735,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="129" spans="2:4" ht="145.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:4" ht="145.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B129" s="4" t="s">
         <v>12</v>
       </c>
@@ -2744,16 +2744,16 @@
       </c>
       <c r="D129" s="12"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B131" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C131" s="14" t="s">
+      <c r="C131" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D131" s="14"/>
-    </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D131" s="13"/>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
         <v>0</v>
       </c>
@@ -2762,7 +2762,7 @@
       </c>
       <c r="D132" s="9"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B133" s="1" t="s">
         <v>8</v>
       </c>
@@ -2771,7 +2771,7 @@
       </c>
       <c r="D133" s="9"/>
     </row>
-    <row r="134" spans="2:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:4" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B134" s="1" t="s">
         <v>9</v>
       </c>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="D134" s="12"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>1</v>
       </c>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="D135" s="9"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B136" s="1" t="s">
         <v>10</v>
       </c>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="D136" s="9"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B137" s="1" t="s">
         <v>2</v>
       </c>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="D137" s="9"/>
     </row>
-    <row r="138" spans="2:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:4" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B138" s="1" t="s">
         <v>3</v>
       </c>
@@ -2816,7 +2816,7 @@
       </c>
       <c r="D138" s="7"/>
     </row>
-    <row r="139" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B139" s="1" t="s">
         <v>4</v>
       </c>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="D139" s="5"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B140" s="10" t="s">
         <v>11</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B141" s="10"/>
       <c r="C141" s="2" t="s">
         <v>142</v>
@@ -2845,7 +2845,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="142" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B142" s="10"/>
       <c r="C142" s="2" t="s">
         <v>144</v>
@@ -2854,7 +2854,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B143" s="10"/>
       <c r="C143" s="2" t="s">
         <v>145</v>
@@ -2863,7 +2863,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="144" spans="2:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B144" s="10"/>
       <c r="C144" s="2" t="s">
         <v>146</v>
@@ -2872,7 +2872,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="145" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B145" s="10"/>
       <c r="C145" s="2" t="s">
         <v>147</v>
@@ -2881,7 +2881,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="146" spans="2:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:4" ht="78" x14ac:dyDescent="0.3">
       <c r="B146" s="10"/>
       <c r="C146" s="2" t="s">
         <v>148</v>
@@ -2890,7 +2890,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="147" spans="2:4" ht="62" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B147" s="10"/>
       <c r="C147" s="2" t="s">
         <v>149</v>
@@ -2899,7 +2899,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="148" spans="2:4" ht="96.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:4" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B148" s="4" t="s">
         <v>12</v>
       </c>
@@ -2910,6 +2910,69 @@
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="B30:B36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="B11:B18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="B48:B54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="B66:B72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="B84:B90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="B102:B108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="B120:B128"/>
+    <mergeCell ref="C129:D129"/>
     <mergeCell ref="C136:D136"/>
     <mergeCell ref="C137:D137"/>
     <mergeCell ref="B140:B147"/>
@@ -2919,69 +2982,6 @@
     <mergeCell ref="C133:D133"/>
     <mergeCell ref="C134:D134"/>
     <mergeCell ref="C135:D135"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="B120:B128"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="B102:B108"/>
-    <mergeCell ref="B84:B90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="B66:B72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B11:B18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="B30:B36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>